<commit_message>
Added thesis paper and graphic folder
</commit_message>
<xml_diff>
--- a/tour_sheets/TourSheet_Thursday.xlsx
+++ b/tour_sheets/TourSheet_Thursday.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="160">
   <si>
     <t>Thursday</t>
   </si>
@@ -496,12 +496,6 @@
   </si>
   <si>
     <t>Frobenius-Forster-Straße 1a</t>
-  </si>
-  <si>
-    <t>Start A</t>
-  </si>
-  <si>
-    <t>End A</t>
   </si>
 </sst>
 </file>
@@ -878,10 +872,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G155"/>
+  <dimension ref="A1:G151"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -895,64 +889,134 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>30</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" s="1"/>
+      <c r="A2" s="4">
+        <v>335</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="6">
+        <v>4903781</v>
+      </c>
+      <c r="E2" s="6">
+        <v>1212439</v>
+      </c>
+      <c r="F2" s="3">
+        <v>1</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="B3">
-        <v>6</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="D3">
-        <v>153</v>
+      <c r="A3" s="4">
+        <v>334</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D3" s="6">
+        <v>4903779</v>
+      </c>
+      <c r="E3" s="6">
+        <v>1212245</v>
+      </c>
+      <c r="F3" s="3">
+        <v>1</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="4">
+        <v>333</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D4" s="6">
+        <v>4903796</v>
+      </c>
+      <c r="E4" s="6">
+        <v>1212088</v>
+      </c>
+      <c r="F4" s="3">
+        <v>1</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>34</v>
+      <c r="A5" s="4">
+        <v>336</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D5" s="6">
+        <v>4903888</v>
+      </c>
+      <c r="E5" s="6">
+        <v>1211562</v>
+      </c>
+      <c r="F5" s="3">
+        <v>1</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="4">
-        <v>335</v>
+        <v>339</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>3</v>
+        <v>40</v>
       </c>
       <c r="D6" s="6">
-        <v>4903781</v>
+        <v>4903951</v>
       </c>
       <c r="E6" s="6">
-        <v>1212439</v>
+        <v>1211449</v>
       </c>
       <c r="F6" s="3">
         <v>1</v>
@@ -962,43 +1026,43 @@
       </c>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="4">
-        <v>334</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="D7" s="6">
-        <v>4903779</v>
-      </c>
-      <c r="E7" s="6">
-        <v>1212245</v>
-      </c>
-      <c r="F7" s="3">
-        <v>1</v>
-      </c>
-      <c r="G7" s="3" t="s">
+      <c r="A7" s="5">
+        <v>115</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D7" s="7">
+        <v>4903951</v>
+      </c>
+      <c r="E7" s="7">
+        <v>1211449</v>
+      </c>
+      <c r="F7" s="2">
+        <v>2</v>
+      </c>
+      <c r="G7" s="2" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="4">
-        <v>333</v>
+        <v>340</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="D8" s="6">
-        <v>4903796</v>
+        <v>4903914</v>
       </c>
       <c r="E8" s="6">
-        <v>1212088</v>
+        <v>1211033</v>
       </c>
       <c r="F8" s="3">
         <v>1</v>
@@ -1008,43 +1072,43 @@
       </c>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="4">
-        <v>336</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="D9" s="6">
-        <v>4903888</v>
-      </c>
-      <c r="E9" s="6">
-        <v>1211562</v>
-      </c>
-      <c r="F9" s="3">
-        <v>1</v>
-      </c>
-      <c r="G9" s="3" t="s">
+      <c r="A9" s="5">
+        <v>118</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D9" s="7">
+        <v>4903942</v>
+      </c>
+      <c r="E9" s="7">
+        <v>1210913</v>
+      </c>
+      <c r="F9" s="2">
+        <v>1</v>
+      </c>
+      <c r="G9" s="2" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="4">
-        <v>339</v>
+        <v>341</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="D10" s="6">
-        <v>4903951</v>
+        <v>4904024</v>
       </c>
       <c r="E10" s="6">
-        <v>1211449</v>
+        <v>1210672</v>
       </c>
       <c r="F10" s="3">
         <v>1</v>
@@ -1054,43 +1118,43 @@
       </c>
     </row>
     <row r="11" spans="1:7">
-      <c r="A11" s="5">
-        <v>115</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D11" s="7">
-        <v>4903951</v>
-      </c>
-      <c r="E11" s="7">
-        <v>1211449</v>
-      </c>
-      <c r="F11" s="2">
-        <v>2</v>
-      </c>
-      <c r="G11" s="2" t="s">
+      <c r="A11" s="4">
+        <v>311</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D11" s="6">
+        <v>4904347</v>
+      </c>
+      <c r="E11" s="6">
+        <v>1210447</v>
+      </c>
+      <c r="F11" s="3">
+        <v>1</v>
+      </c>
+      <c r="G11" s="3" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="4">
-        <v>340</v>
+        <v>310</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="D12" s="6">
-        <v>4903914</v>
+        <v>4904417</v>
       </c>
       <c r="E12" s="6">
-        <v>1211033</v>
+        <v>1210344</v>
       </c>
       <c r="F12" s="3">
         <v>1</v>
@@ -1100,43 +1164,43 @@
       </c>
     </row>
     <row r="13" spans="1:7">
-      <c r="A13" s="5">
-        <v>118</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="D13" s="7">
-        <v>4903942</v>
-      </c>
-      <c r="E13" s="7">
-        <v>1210913</v>
-      </c>
-      <c r="F13" s="2">
-        <v>1</v>
-      </c>
-      <c r="G13" s="2" t="s">
+      <c r="A13" s="4">
+        <v>342</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D13" s="6">
+        <v>4904257</v>
+      </c>
+      <c r="E13" s="6">
+        <v>1210237</v>
+      </c>
+      <c r="F13" s="3">
+        <v>1</v>
+      </c>
+      <c r="G13" s="3" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="4">
-        <v>341</v>
+        <v>343</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="D14" s="6">
-        <v>4904024</v>
+        <v>4904065</v>
       </c>
       <c r="E14" s="6">
-        <v>1210672</v>
+        <v>1210387</v>
       </c>
       <c r="F14" s="3">
         <v>1</v>
@@ -1147,19 +1211,19 @@
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="4">
-        <v>311</v>
+        <v>345</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="D15" s="6">
-        <v>4904347</v>
+        <v>4903920</v>
       </c>
       <c r="E15" s="6">
-        <v>1210447</v>
+        <v>1210332</v>
       </c>
       <c r="F15" s="3">
         <v>1</v>
@@ -1170,19 +1234,19 @@
     </row>
     <row r="16" spans="1:7">
       <c r="A16" s="4">
-        <v>310</v>
+        <v>344</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="D16" s="6">
-        <v>4904417</v>
+        <v>4903839</v>
       </c>
       <c r="E16" s="6">
-        <v>1210344</v>
+        <v>1210737</v>
       </c>
       <c r="F16" s="3">
         <v>1</v>
@@ -1193,19 +1257,19 @@
     </row>
     <row r="17" spans="1:7">
       <c r="A17" s="4">
-        <v>342</v>
+        <v>367</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="D17" s="6">
-        <v>4904257</v>
+        <v>4903732</v>
       </c>
       <c r="E17" s="6">
-        <v>1210237</v>
+        <v>1211061</v>
       </c>
       <c r="F17" s="3">
         <v>1</v>
@@ -1216,19 +1280,19 @@
     </row>
     <row r="18" spans="1:7">
       <c r="A18" s="4">
-        <v>343</v>
+        <v>366</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="D18" s="6">
-        <v>4904065</v>
+        <v>4903572</v>
       </c>
       <c r="E18" s="6">
-        <v>1210387</v>
+        <v>1211448</v>
       </c>
       <c r="F18" s="3">
         <v>1</v>
@@ -1238,43 +1302,43 @@
       </c>
     </row>
     <row r="19" spans="1:7">
-      <c r="A19" s="4">
-        <v>345</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="D19" s="6">
-        <v>4903920</v>
-      </c>
-      <c r="E19" s="6">
-        <v>1210332</v>
-      </c>
-      <c r="F19" s="3">
-        <v>1</v>
-      </c>
-      <c r="G19" s="3" t="s">
+      <c r="A19" s="5">
+        <v>221</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="D19" s="7">
+        <v>4903430</v>
+      </c>
+      <c r="E19" s="7">
+        <v>1211451</v>
+      </c>
+      <c r="F19" s="2">
+        <v>3</v>
+      </c>
+      <c r="G19" s="2" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:7">
       <c r="A20" s="4">
-        <v>344</v>
+        <v>365</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="D20" s="6">
-        <v>4903839</v>
+        <v>4903669</v>
       </c>
       <c r="E20" s="6">
-        <v>1210737</v>
+        <v>1211665</v>
       </c>
       <c r="F20" s="3">
         <v>1</v>
@@ -1285,19 +1349,19 @@
     </row>
     <row r="21" spans="1:7">
       <c r="A21" s="4">
-        <v>367</v>
+        <v>330</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="D21" s="6">
-        <v>4903732</v>
+        <v>4904026</v>
       </c>
       <c r="E21" s="6">
-        <v>1211061</v>
+        <v>1212552</v>
       </c>
       <c r="F21" s="3">
         <v>1</v>
@@ -1308,19 +1372,19 @@
     </row>
     <row r="22" spans="1:7">
       <c r="A22" s="4">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="D22" s="6">
-        <v>4903572</v>
+        <v>4903714</v>
       </c>
       <c r="E22" s="6">
-        <v>1211448</v>
+        <v>1212747</v>
       </c>
       <c r="F22" s="3">
         <v>1</v>
@@ -1331,22 +1395,22 @@
     </row>
     <row r="23" spans="1:7">
       <c r="A23" s="5">
-        <v>221</v>
+        <v>83</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>151</v>
+        <v>56</v>
       </c>
       <c r="D23" s="7">
-        <v>4903430</v>
+        <v>4903988</v>
       </c>
       <c r="E23" s="7">
-        <v>1211451</v>
+        <v>1212655</v>
       </c>
       <c r="F23" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G23" s="2" t="s">
         <v>0</v>
@@ -1354,19 +1418,19 @@
     </row>
     <row r="24" spans="1:7">
       <c r="A24" s="4">
-        <v>365</v>
+        <v>329</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="D24" s="6">
-        <v>4903669</v>
+        <v>4903929</v>
       </c>
       <c r="E24" s="6">
-        <v>1211665</v>
+        <v>1212677</v>
       </c>
       <c r="F24" s="3">
         <v>1</v>
@@ -1377,19 +1441,19 @@
     </row>
     <row r="25" spans="1:7">
       <c r="A25" s="4">
-        <v>330</v>
+        <v>361</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="D25" s="6">
-        <v>4904026</v>
+        <v>4903714</v>
       </c>
       <c r="E25" s="6">
-        <v>1212552</v>
+        <v>1212511</v>
       </c>
       <c r="F25" s="3">
         <v>1</v>
@@ -1399,66 +1463,66 @@
       </c>
     </row>
     <row r="26" spans="1:7">
-      <c r="A26" s="4">
-        <v>362</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="D26" s="6">
-        <v>4903714</v>
-      </c>
-      <c r="E26" s="6">
-        <v>1212747</v>
-      </c>
-      <c r="F26" s="3">
-        <v>1</v>
-      </c>
-      <c r="G26" s="3" t="s">
+      <c r="A26" s="5">
+        <v>84</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D26" s="7">
+        <v>4904104</v>
+      </c>
+      <c r="E26" s="7">
+        <v>1212232</v>
+      </c>
+      <c r="F26" s="2">
+        <v>1</v>
+      </c>
+      <c r="G26" s="2" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:7">
-      <c r="A27" s="5">
-        <v>83</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="D27" s="7">
-        <v>4903988</v>
-      </c>
-      <c r="E27" s="7">
-        <v>1212655</v>
-      </c>
-      <c r="F27" s="2">
-        <v>1</v>
-      </c>
-      <c r="G27" s="2" t="s">
+      <c r="A27" s="4">
+        <v>454</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D27" s="6">
+        <v>4904158</v>
+      </c>
+      <c r="E27" s="6">
+        <v>1212096</v>
+      </c>
+      <c r="F27" s="3">
+        <v>1</v>
+      </c>
+      <c r="G27" s="3" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:7">
       <c r="A28" s="4">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="D28" s="6">
-        <v>4903929</v>
+        <v>4904113</v>
       </c>
       <c r="E28" s="6">
-        <v>1212677</v>
+        <v>1212319</v>
       </c>
       <c r="F28" s="3">
         <v>1</v>
@@ -1469,19 +1533,19 @@
     </row>
     <row r="29" spans="1:7">
       <c r="A29" s="4">
-        <v>361</v>
+        <v>332</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="D29" s="6">
-        <v>4903714</v>
+        <v>4903917</v>
       </c>
       <c r="E29" s="6">
-        <v>1212511</v>
+        <v>1212156</v>
       </c>
       <c r="F29" s="3">
         <v>1</v>
@@ -1491,43 +1555,43 @@
       </c>
     </row>
     <row r="30" spans="1:7">
-      <c r="A30" s="5">
-        <v>84</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="D30" s="7">
-        <v>4904104</v>
-      </c>
-      <c r="E30" s="7">
-        <v>1212232</v>
-      </c>
-      <c r="F30" s="2">
-        <v>1</v>
-      </c>
-      <c r="G30" s="2" t="s">
+      <c r="A30" s="4">
+        <v>337</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D30" s="6">
+        <v>4903972</v>
+      </c>
+      <c r="E30" s="6">
+        <v>1211824</v>
+      </c>
+      <c r="F30" s="3">
+        <v>1</v>
+      </c>
+      <c r="G30" s="3" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:7">
       <c r="A31" s="4">
-        <v>454</v>
+        <v>338</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="D31" s="6">
-        <v>4904158</v>
+        <v>4904105</v>
       </c>
       <c r="E31" s="6">
-        <v>1212096</v>
+        <v>1211656</v>
       </c>
       <c r="F31" s="3">
         <v>1</v>
@@ -1538,19 +1602,19 @@
     </row>
     <row r="32" spans="1:7">
       <c r="A32" s="4">
-        <v>331</v>
+        <v>312</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="D32" s="6">
-        <v>4904113</v>
+        <v>4904424</v>
       </c>
       <c r="E32" s="6">
-        <v>1212319</v>
+        <v>1211703</v>
       </c>
       <c r="F32" s="3">
         <v>1</v>
@@ -1561,19 +1625,19 @@
     </row>
     <row r="33" spans="1:7">
       <c r="A33" s="4">
-        <v>332</v>
+        <v>300</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="D33" s="6">
-        <v>4903917</v>
+        <v>4904706</v>
       </c>
       <c r="E33" s="6">
-        <v>1212156</v>
+        <v>1211704</v>
       </c>
       <c r="F33" s="3">
         <v>1</v>
@@ -1584,19 +1648,19 @@
     </row>
     <row r="34" spans="1:7">
       <c r="A34" s="4">
-        <v>337</v>
+        <v>301</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="D34" s="6">
-        <v>4903972</v>
+        <v>4904959</v>
       </c>
       <c r="E34" s="6">
-        <v>1211824</v>
+        <v>1212169</v>
       </c>
       <c r="F34" s="3">
         <v>1</v>
@@ -1607,19 +1671,19 @@
     </row>
     <row r="35" spans="1:7">
       <c r="A35" s="4">
-        <v>338</v>
+        <v>487</v>
       </c>
       <c r="B35" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="D35" s="6">
-        <v>4904105</v>
+        <v>4904861</v>
       </c>
       <c r="E35" s="6">
-        <v>1211656</v>
+        <v>1211908</v>
       </c>
       <c r="F35" s="3">
         <v>1</v>
@@ -1630,19 +1694,19 @@
     </row>
     <row r="36" spans="1:7">
       <c r="A36" s="4">
-        <v>312</v>
+        <v>295</v>
       </c>
       <c r="B36" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="D36" s="6">
-        <v>4904424</v>
+        <v>4904717</v>
       </c>
       <c r="E36" s="6">
-        <v>1211703</v>
+        <v>1211213</v>
       </c>
       <c r="F36" s="3">
         <v>1</v>
@@ -1653,19 +1717,19 @@
     </row>
     <row r="37" spans="1:7">
       <c r="A37" s="4">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="B37" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>66</v>
+        <v>4</v>
       </c>
       <c r="D37" s="6">
-        <v>4904706</v>
+        <v>4904738</v>
       </c>
       <c r="E37" s="6">
-        <v>1211704</v>
+        <v>1210768</v>
       </c>
       <c r="F37" s="3">
         <v>1</v>
@@ -1676,19 +1740,19 @@
     </row>
     <row r="38" spans="1:7">
       <c r="A38" s="4">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="B38" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>67</v>
+        <v>5</v>
       </c>
       <c r="D38" s="6">
-        <v>4904959</v>
+        <v>4904710</v>
       </c>
       <c r="E38" s="6">
-        <v>1212169</v>
+        <v>1210354</v>
       </c>
       <c r="F38" s="3">
         <v>1</v>
@@ -1699,19 +1763,19 @@
     </row>
     <row r="39" spans="1:7">
       <c r="A39" s="4">
-        <v>487</v>
+        <v>298</v>
       </c>
       <c r="B39" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>68</v>
+        <v>6</v>
       </c>
       <c r="D39" s="6">
-        <v>4904861</v>
+        <v>4904870</v>
       </c>
       <c r="E39" s="6">
-        <v>1211908</v>
+        <v>1210436</v>
       </c>
       <c r="F39" s="3">
         <v>1</v>
@@ -1722,19 +1786,19 @@
     </row>
     <row r="40" spans="1:7">
       <c r="A40" s="4">
-        <v>295</v>
+        <v>299</v>
       </c>
       <c r="B40" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>69</v>
+        <v>7</v>
       </c>
       <c r="D40" s="6">
-        <v>4904717</v>
+        <v>4904682</v>
       </c>
       <c r="E40" s="6">
-        <v>1211213</v>
+        <v>1209921</v>
       </c>
       <c r="F40" s="3">
         <v>1</v>
@@ -1745,19 +1809,19 @@
     </row>
     <row r="41" spans="1:7">
       <c r="A41" s="4">
-        <v>296</v>
+        <v>307</v>
       </c>
       <c r="B41" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D41" s="6">
-        <v>4904738</v>
+        <v>4904698</v>
       </c>
       <c r="E41" s="6">
-        <v>1210768</v>
+        <v>1212377</v>
       </c>
       <c r="F41" s="3">
         <v>1</v>
@@ -1768,19 +1832,19 @@
     </row>
     <row r="42" spans="1:7">
       <c r="A42" s="4">
-        <v>297</v>
+        <v>488</v>
       </c>
       <c r="B42" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="D42" s="6">
-        <v>4904710</v>
+        <v>4904728</v>
       </c>
       <c r="E42" s="6">
-        <v>1210354</v>
+        <v>1212655</v>
       </c>
       <c r="F42" s="3">
         <v>1</v>
@@ -1791,19 +1855,19 @@
     </row>
     <row r="43" spans="1:7">
       <c r="A43" s="4">
-        <v>298</v>
+        <v>306</v>
       </c>
       <c r="B43" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D43" s="6">
-        <v>4904870</v>
+        <v>4904714</v>
       </c>
       <c r="E43" s="6">
-        <v>1210436</v>
+        <v>1212595</v>
       </c>
       <c r="F43" s="3">
         <v>1</v>
@@ -1814,19 +1878,19 @@
     </row>
     <row r="44" spans="1:7">
       <c r="A44" s="4">
-        <v>299</v>
+        <v>305</v>
       </c>
       <c r="B44" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D44" s="6">
-        <v>4904682</v>
+        <v>4904738</v>
       </c>
       <c r="E44" s="6">
-        <v>1209921</v>
+        <v>1212957</v>
       </c>
       <c r="F44" s="3">
         <v>1</v>
@@ -1837,19 +1901,19 @@
     </row>
     <row r="45" spans="1:7">
       <c r="A45" s="4">
-        <v>307</v>
+        <v>302</v>
       </c>
       <c r="B45" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>8</v>
+        <v>70</v>
       </c>
       <c r="D45" s="6">
-        <v>4904698</v>
+        <v>4904841</v>
       </c>
       <c r="E45" s="6">
-        <v>1212377</v>
+        <v>1212687</v>
       </c>
       <c r="F45" s="3">
         <v>1</v>
@@ -1860,19 +1924,19 @@
     </row>
     <row r="46" spans="1:7">
       <c r="A46" s="4">
-        <v>488</v>
+        <v>303</v>
       </c>
       <c r="B46" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>11</v>
+        <v>71</v>
       </c>
       <c r="D46" s="6">
-        <v>4904728</v>
+        <v>4904847</v>
       </c>
       <c r="E46" s="6">
-        <v>1212655</v>
+        <v>1212595</v>
       </c>
       <c r="F46" s="3">
         <v>1</v>
@@ -1883,19 +1947,19 @@
     </row>
     <row r="47" spans="1:7">
       <c r="A47" s="4">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="B47" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>9</v>
+        <v>72</v>
       </c>
       <c r="D47" s="6">
-        <v>4904714</v>
+        <v>4905031</v>
       </c>
       <c r="E47" s="6">
-        <v>1212595</v>
+        <v>1212523</v>
       </c>
       <c r="F47" s="3">
         <v>1</v>
@@ -1905,43 +1969,43 @@
       </c>
     </row>
     <row r="48" spans="1:7">
-      <c r="A48" s="4">
-        <v>305</v>
-      </c>
-      <c r="B48" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C48" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D48" s="6">
-        <v>4904738</v>
-      </c>
-      <c r="E48" s="6">
-        <v>1212957</v>
-      </c>
-      <c r="F48" s="3">
-        <v>1</v>
-      </c>
-      <c r="G48" s="3" t="s">
+      <c r="A48" s="5">
+        <v>3</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D48" s="7">
+        <v>4905057</v>
+      </c>
+      <c r="E48" s="7">
+        <v>1212486</v>
+      </c>
+      <c r="F48" s="2">
+        <v>1</v>
+      </c>
+      <c r="G48" s="2" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="49" spans="1:7">
       <c r="A49" s="4">
-        <v>302</v>
+        <v>320</v>
       </c>
       <c r="B49" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="D49" s="6">
-        <v>4904841</v>
+        <v>4904427</v>
       </c>
       <c r="E49" s="6">
-        <v>1212687</v>
+        <v>1212841</v>
       </c>
       <c r="F49" s="3">
         <v>1</v>
@@ -1952,19 +2016,19 @@
     </row>
     <row r="50" spans="1:7">
       <c r="A50" s="4">
-        <v>303</v>
+        <v>328</v>
       </c>
       <c r="B50" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="D50" s="6">
-        <v>4904847</v>
+        <v>4904033</v>
       </c>
       <c r="E50" s="6">
-        <v>1212595</v>
+        <v>1212879</v>
       </c>
       <c r="F50" s="3">
         <v>1</v>
@@ -1975,19 +2039,19 @@
     </row>
     <row r="51" spans="1:7">
       <c r="A51" s="4">
-        <v>304</v>
+        <v>326</v>
       </c>
       <c r="B51" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="D51" s="6">
-        <v>4905031</v>
+        <v>4903931</v>
       </c>
       <c r="E51" s="6">
-        <v>1212523</v>
+        <v>1213226</v>
       </c>
       <c r="F51" s="3">
         <v>1</v>
@@ -1997,43 +2061,43 @@
       </c>
     </row>
     <row r="52" spans="1:7">
-      <c r="A52" s="5">
-        <v>3</v>
-      </c>
-      <c r="B52" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C52" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="D52" s="7">
-        <v>4905057</v>
-      </c>
-      <c r="E52" s="7">
-        <v>1212486</v>
-      </c>
-      <c r="F52" s="2">
-        <v>1</v>
-      </c>
-      <c r="G52" s="2" t="s">
+      <c r="A52" s="4">
+        <v>327</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="D52" s="6">
+        <v>4904155</v>
+      </c>
+      <c r="E52" s="6">
+        <v>1213198</v>
+      </c>
+      <c r="F52" s="3">
+        <v>1</v>
+      </c>
+      <c r="G52" s="3" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="53" spans="1:7">
       <c r="A53" s="4">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="B53" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="D53" s="6">
-        <v>4904427</v>
+        <v>4904372</v>
       </c>
       <c r="E53" s="6">
-        <v>1212841</v>
+        <v>1213157</v>
       </c>
       <c r="F53" s="3">
         <v>1</v>
@@ -2044,19 +2108,19 @@
     </row>
     <row r="54" spans="1:7">
       <c r="A54" s="4">
-        <v>328</v>
+        <v>323</v>
       </c>
       <c r="B54" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="D54" s="6">
-        <v>4904033</v>
+        <v>4904507</v>
       </c>
       <c r="E54" s="6">
-        <v>1212879</v>
+        <v>1213102</v>
       </c>
       <c r="F54" s="3">
         <v>1</v>
@@ -2067,19 +2131,19 @@
     </row>
     <row r="55" spans="1:7">
       <c r="A55" s="4">
-        <v>326</v>
+        <v>321</v>
       </c>
       <c r="B55" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="D55" s="6">
-        <v>4903931</v>
+        <v>4904256</v>
       </c>
       <c r="E55" s="6">
-        <v>1213226</v>
+        <v>1213027</v>
       </c>
       <c r="F55" s="3">
         <v>1</v>
@@ -2090,19 +2154,19 @@
     </row>
     <row r="56" spans="1:7">
       <c r="A56" s="4">
-        <v>327</v>
+        <v>318</v>
       </c>
       <c r="B56" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="D56" s="6">
-        <v>4904155</v>
+        <v>4904374</v>
       </c>
       <c r="E56" s="6">
-        <v>1213198</v>
+        <v>1212594</v>
       </c>
       <c r="F56" s="3">
         <v>1</v>
@@ -2113,19 +2177,19 @@
     </row>
     <row r="57" spans="1:7">
       <c r="A57" s="4">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="B57" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="D57" s="6">
-        <v>4904372</v>
+        <v>4904586</v>
       </c>
       <c r="E57" s="6">
-        <v>1213157</v>
+        <v>1212735</v>
       </c>
       <c r="F57" s="3">
         <v>1</v>
@@ -2136,19 +2200,19 @@
     </row>
     <row r="58" spans="1:7">
       <c r="A58" s="4">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="B58" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="D58" s="6">
-        <v>4904507</v>
+        <v>4903694</v>
       </c>
       <c r="E58" s="6">
-        <v>1213102</v>
+        <v>1213186</v>
       </c>
       <c r="F58" s="3">
         <v>1</v>
@@ -2159,19 +2223,19 @@
     </row>
     <row r="59" spans="1:7">
       <c r="A59" s="4">
-        <v>321</v>
+        <v>360</v>
       </c>
       <c r="B59" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="D59" s="6">
-        <v>4904256</v>
+        <v>4903596</v>
       </c>
       <c r="E59" s="6">
-        <v>1213027</v>
+        <v>1212859</v>
       </c>
       <c r="F59" s="3">
         <v>1</v>
@@ -2181,89 +2245,89 @@
       </c>
     </row>
     <row r="60" spans="1:7">
-      <c r="A60" s="4">
-        <v>318</v>
-      </c>
-      <c r="B60" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C60" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="D60" s="6">
-        <v>4904374</v>
-      </c>
-      <c r="E60" s="6">
-        <v>1212594</v>
-      </c>
-      <c r="F60" s="3">
-        <v>1</v>
-      </c>
-      <c r="G60" s="3" t="s">
+      <c r="A60" s="5">
+        <v>209</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D60" s="7">
+        <v>4903596</v>
+      </c>
+      <c r="E60" s="7">
+        <v>1212814</v>
+      </c>
+      <c r="F60" s="2">
+        <v>2</v>
+      </c>
+      <c r="G60" s="2" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="61" spans="1:7">
-      <c r="A61" s="4">
-        <v>319</v>
-      </c>
-      <c r="B61" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C61" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="D61" s="6">
-        <v>4904586</v>
-      </c>
-      <c r="E61" s="6">
-        <v>1212735</v>
-      </c>
-      <c r="F61" s="3">
-        <v>1</v>
-      </c>
-      <c r="G61" s="3" t="s">
+      <c r="A61" s="5">
+        <v>223</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D61" s="7">
+        <v>4903518</v>
+      </c>
+      <c r="E61" s="7">
+        <v>1212228</v>
+      </c>
+      <c r="F61" s="2">
+        <v>1</v>
+      </c>
+      <c r="G61" s="2" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="62" spans="1:7">
-      <c r="A62" s="4">
-        <v>325</v>
-      </c>
-      <c r="B62" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C62" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="D62" s="6">
-        <v>4903694</v>
-      </c>
-      <c r="E62" s="6">
-        <v>1213186</v>
-      </c>
-      <c r="F62" s="3">
-        <v>1</v>
-      </c>
-      <c r="G62" s="3" t="s">
+      <c r="A62" s="5">
+        <v>210</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D62" s="7">
+        <v>4903343</v>
+      </c>
+      <c r="E62" s="7">
+        <v>1211832</v>
+      </c>
+      <c r="F62" s="2">
+        <v>1</v>
+      </c>
+      <c r="G62" s="2" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="63" spans="1:7">
       <c r="A63" s="4">
-        <v>360</v>
+        <v>363</v>
       </c>
       <c r="B63" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="D63" s="6">
-        <v>4903596</v>
+        <v>4903551</v>
       </c>
       <c r="E63" s="6">
-        <v>1212859</v>
+        <v>1212184</v>
       </c>
       <c r="F63" s="3">
         <v>1</v>
@@ -2274,134 +2338,134 @@
     </row>
     <row r="64" spans="1:7">
       <c r="A64" s="5">
-        <v>209</v>
+        <v>197</v>
       </c>
       <c r="B64" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="D64" s="7">
-        <v>4903596</v>
+        <v>4903335</v>
       </c>
       <c r="E64" s="7">
-        <v>1212814</v>
+        <v>1212069</v>
       </c>
       <c r="F64" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G64" s="2" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="65" spans="1:7">
-      <c r="A65" s="5">
-        <v>223</v>
-      </c>
-      <c r="B65" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C65" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="D65" s="7">
-        <v>4903518</v>
-      </c>
-      <c r="E65" s="7">
-        <v>1212228</v>
-      </c>
-      <c r="F65" s="2">
-        <v>1</v>
-      </c>
-      <c r="G65" s="2" t="s">
+      <c r="A65" s="4">
+        <v>364</v>
+      </c>
+      <c r="B65" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C65" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D65" s="6">
+        <v>4903515</v>
+      </c>
+      <c r="E65" s="6">
+        <v>1211691</v>
+      </c>
+      <c r="F65" s="3">
+        <v>1</v>
+      </c>
+      <c r="G65" s="3" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="66" spans="1:7">
       <c r="A66" s="5">
-        <v>210</v>
+        <v>222</v>
       </c>
       <c r="B66" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="D66" s="7">
-        <v>4903343</v>
+        <v>4903373</v>
       </c>
       <c r="E66" s="7">
-        <v>1211832</v>
+        <v>1212199</v>
       </c>
       <c r="F66" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G66" s="2" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="67" spans="1:7">
-      <c r="A67" s="4">
-        <v>363</v>
-      </c>
-      <c r="B67" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C67" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="D67" s="6">
-        <v>4903551</v>
-      </c>
-      <c r="E67" s="6">
-        <v>1212184</v>
-      </c>
-      <c r="F67" s="3">
-        <v>1</v>
-      </c>
-      <c r="G67" s="3" t="s">
+      <c r="A67" s="5">
+        <v>138</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C67" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="D67" s="7">
+        <v>4903352</v>
+      </c>
+      <c r="E67" s="7">
+        <v>1212557</v>
+      </c>
+      <c r="F67" s="2">
+        <v>2</v>
+      </c>
+      <c r="G67" s="2" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="68" spans="1:7">
-      <c r="A68" s="5">
-        <v>197</v>
-      </c>
-      <c r="B68" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C68" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="D68" s="7">
-        <v>4903335</v>
-      </c>
-      <c r="E68" s="7">
-        <v>1212069</v>
-      </c>
-      <c r="F68" s="2">
-        <v>1</v>
-      </c>
-      <c r="G68" s="2" t="s">
+      <c r="A68" s="4">
+        <v>465</v>
+      </c>
+      <c r="B68" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C68" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="D68" s="6">
+        <v>4903380</v>
+      </c>
+      <c r="E68" s="6">
+        <v>1211786</v>
+      </c>
+      <c r="F68" s="3">
+        <v>1</v>
+      </c>
+      <c r="G68" s="3" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="69" spans="1:7">
       <c r="A69" s="4">
-        <v>364</v>
+        <v>466</v>
       </c>
       <c r="B69" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="D69" s="6">
-        <v>4903515</v>
+        <v>4903382</v>
       </c>
       <c r="E69" s="6">
-        <v>1211691</v>
+        <v>1212464</v>
       </c>
       <c r="F69" s="3">
         <v>1</v>
@@ -2412,22 +2476,22 @@
     </row>
     <row r="70" spans="1:7">
       <c r="A70" s="5">
-        <v>222</v>
+        <v>140</v>
       </c>
       <c r="B70" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="D70" s="7">
-        <v>4903373</v>
+        <v>4903333</v>
       </c>
       <c r="E70" s="7">
-        <v>1212199</v>
+        <v>1212612</v>
       </c>
       <c r="F70" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G70" s="2" t="s">
         <v>0</v>
@@ -2435,88 +2499,88 @@
     </row>
     <row r="71" spans="1:7">
       <c r="A71" s="5">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="B71" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="D71" s="7">
-        <v>4903352</v>
+        <v>4903323</v>
       </c>
       <c r="E71" s="7">
-        <v>1212557</v>
+        <v>1212612</v>
       </c>
       <c r="F71" s="2">
+        <v>1</v>
+      </c>
+      <c r="G71" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7">
+      <c r="A72" s="5">
+        <v>142</v>
+      </c>
+      <c r="B72" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="G71" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="72" spans="1:7">
-      <c r="A72" s="4">
-        <v>465</v>
-      </c>
-      <c r="B72" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C72" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="D72" s="6">
-        <v>4903380</v>
-      </c>
-      <c r="E72" s="6">
-        <v>1211786</v>
-      </c>
-      <c r="F72" s="3">
-        <v>1</v>
-      </c>
-      <c r="G72" s="3" t="s">
+      <c r="C72" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D72" s="7">
+        <v>4903285</v>
+      </c>
+      <c r="E72" s="7">
+        <v>1212614</v>
+      </c>
+      <c r="F72" s="2">
+        <v>1</v>
+      </c>
+      <c r="G72" s="2" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="73" spans="1:7">
-      <c r="A73" s="4">
-        <v>466</v>
-      </c>
-      <c r="B73" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C73" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="D73" s="6">
-        <v>4903382</v>
-      </c>
-      <c r="E73" s="6">
-        <v>1212464</v>
-      </c>
-      <c r="F73" s="3">
-        <v>1</v>
-      </c>
-      <c r="G73" s="3" t="s">
+      <c r="A73" s="5">
+        <v>300</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C73" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="D73" s="7">
+        <v>4903391</v>
+      </c>
+      <c r="E73" s="7">
+        <v>1212572</v>
+      </c>
+      <c r="F73" s="2">
+        <v>1</v>
+      </c>
+      <c r="G73" s="2" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="74" spans="1:7">
       <c r="A74" s="5">
-        <v>140</v>
+        <v>198</v>
       </c>
       <c r="B74" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="D74" s="7">
-        <v>4903333</v>
+        <v>4903334</v>
       </c>
       <c r="E74" s="7">
-        <v>1212612</v>
+        <v>1212024</v>
       </c>
       <c r="F74" s="2">
         <v>1</v>
@@ -2527,19 +2591,19 @@
     </row>
     <row r="75" spans="1:7">
       <c r="A75" s="5">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B75" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="D75" s="7">
-        <v>4903323</v>
+        <v>4903392</v>
       </c>
       <c r="E75" s="7">
-        <v>1212612</v>
+        <v>1212674</v>
       </c>
       <c r="F75" s="2">
         <v>1</v>
@@ -2550,19 +2614,19 @@
     </row>
     <row r="76" spans="1:7">
       <c r="A76" s="5">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B76" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="D76" s="7">
-        <v>4903285</v>
+        <v>4903342</v>
       </c>
       <c r="E76" s="7">
-        <v>1212614</v>
+        <v>1212794</v>
       </c>
       <c r="F76" s="2">
         <v>1</v>
@@ -2573,19 +2637,19 @@
     </row>
     <row r="77" spans="1:7">
       <c r="A77" s="5">
-        <v>300</v>
+        <v>144</v>
       </c>
       <c r="B77" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="D77" s="7">
-        <v>4903391</v>
+        <v>4903317</v>
       </c>
       <c r="E77" s="7">
-        <v>1212572</v>
+        <v>1212839</v>
       </c>
       <c r="F77" s="2">
         <v>1</v>
@@ -2596,19 +2660,19 @@
     </row>
     <row r="78" spans="1:7">
       <c r="A78" s="5">
-        <v>198</v>
+        <v>146</v>
       </c>
       <c r="B78" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="D78" s="7">
-        <v>4903334</v>
+        <v>4903345</v>
       </c>
       <c r="E78" s="7">
-        <v>1212024</v>
+        <v>1213030</v>
       </c>
       <c r="F78" s="2">
         <v>1</v>
@@ -2619,91 +2683,91 @@
     </row>
     <row r="79" spans="1:7">
       <c r="A79" s="5">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="B79" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="D79" s="7">
-        <v>4903392</v>
+        <v>4903403</v>
       </c>
       <c r="E79" s="7">
-        <v>1212674</v>
+        <v>1212938</v>
       </c>
       <c r="F79" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G79" s="2" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="80" spans="1:7">
-      <c r="A80" s="5">
-        <v>143</v>
-      </c>
-      <c r="B80" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C80" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="D80" s="7">
-        <v>4903342</v>
-      </c>
-      <c r="E80" s="7">
-        <v>1212794</v>
-      </c>
-      <c r="F80" s="2">
-        <v>1</v>
-      </c>
-      <c r="G80" s="2" t="s">
+      <c r="A80" s="4">
+        <v>316</v>
+      </c>
+      <c r="B80" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C80" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="D80" s="6">
+        <v>4904237</v>
+      </c>
+      <c r="E80" s="6">
+        <v>1212349</v>
+      </c>
+      <c r="F80" s="3">
+        <v>1</v>
+      </c>
+      <c r="G80" s="3" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="81" spans="1:7">
-      <c r="A81" s="5">
-        <v>144</v>
-      </c>
-      <c r="B81" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C81" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="D81" s="7">
-        <v>4903317</v>
-      </c>
-      <c r="E81" s="7">
-        <v>1212839</v>
-      </c>
-      <c r="F81" s="2">
-        <v>1</v>
-      </c>
-      <c r="G81" s="2" t="s">
+      <c r="A81" s="4">
+        <v>315</v>
+      </c>
+      <c r="B81" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C81" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D81" s="6">
+        <v>4904414</v>
+      </c>
+      <c r="E81" s="6">
+        <v>1212142</v>
+      </c>
+      <c r="F81" s="3">
+        <v>1</v>
+      </c>
+      <c r="G81" s="3" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="82" spans="1:7">
       <c r="A82" s="5">
-        <v>146</v>
+        <v>249</v>
       </c>
       <c r="B82" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="D82" s="7">
-        <v>4903345</v>
+        <v>4904538</v>
       </c>
       <c r="E82" s="7">
-        <v>1213030</v>
+        <v>1212218</v>
       </c>
       <c r="F82" s="2">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G82" s="2" t="s">
         <v>0</v>
@@ -2711,65 +2775,65 @@
     </row>
     <row r="83" spans="1:7">
       <c r="A83" s="5">
-        <v>145</v>
+        <v>247</v>
       </c>
       <c r="B83" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="D83" s="7">
-        <v>4903403</v>
+        <v>4904752</v>
       </c>
       <c r="E83" s="7">
-        <v>1212938</v>
+        <v>1211927</v>
       </c>
       <c r="F83" s="2">
+        <v>1</v>
+      </c>
+      <c r="G83" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7">
+      <c r="A84" s="5">
+        <v>304</v>
+      </c>
+      <c r="B84" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="G83" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="84" spans="1:7">
-      <c r="A84" s="4">
-        <v>316</v>
-      </c>
-      <c r="B84" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C84" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="D84" s="6">
-        <v>4904237</v>
-      </c>
-      <c r="E84" s="6">
-        <v>1212349</v>
-      </c>
-      <c r="F84" s="3">
-        <v>1</v>
-      </c>
-      <c r="G84" s="3" t="s">
+      <c r="C84" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D84" s="7">
+        <v>4904695</v>
+      </c>
+      <c r="E84" s="7">
+        <v>1211845</v>
+      </c>
+      <c r="F84" s="2">
+        <v>1</v>
+      </c>
+      <c r="G84" s="2" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="85" spans="1:7">
       <c r="A85" s="4">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="B85" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C85" s="3" t="s">
-        <v>12</v>
+        <v>109</v>
       </c>
       <c r="D85" s="6">
-        <v>4904414</v>
+        <v>4904423</v>
       </c>
       <c r="E85" s="6">
-        <v>1212142</v>
+        <v>1211864</v>
       </c>
       <c r="F85" s="3">
         <v>1</v>
@@ -2780,68 +2844,68 @@
     </row>
     <row r="86" spans="1:7">
       <c r="A86" s="5">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B86" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="D86" s="7">
-        <v>4904538</v>
+        <v>4904649</v>
       </c>
       <c r="E86" s="7">
-        <v>1212218</v>
+        <v>1211985</v>
       </c>
       <c r="F86" s="2">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="G86" s="2" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="87" spans="1:7">
-      <c r="A87" s="5">
-        <v>247</v>
-      </c>
-      <c r="B87" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C87" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="D87" s="7">
-        <v>4904752</v>
-      </c>
-      <c r="E87" s="7">
-        <v>1211927</v>
-      </c>
-      <c r="F87" s="2">
-        <v>1</v>
-      </c>
-      <c r="G87" s="2" t="s">
+      <c r="A87" s="4">
+        <v>314</v>
+      </c>
+      <c r="B87" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C87" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="D87" s="6">
+        <v>4904349</v>
+      </c>
+      <c r="E87" s="6">
+        <v>1212388</v>
+      </c>
+      <c r="F87" s="3">
+        <v>1</v>
+      </c>
+      <c r="G87" s="3" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="88" spans="1:7">
       <c r="A88" s="5">
-        <v>304</v>
+        <v>58</v>
       </c>
       <c r="B88" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="D88" s="7">
-        <v>4904695</v>
+        <v>4904685</v>
       </c>
       <c r="E88" s="7">
-        <v>1211845</v>
+        <v>1212198</v>
       </c>
       <c r="F88" s="2">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G88" s="2" t="s">
         <v>0</v>
@@ -2849,19 +2913,19 @@
     </row>
     <row r="89" spans="1:7">
       <c r="A89" s="4">
-        <v>313</v>
+        <v>317</v>
       </c>
       <c r="B89" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C89" s="3" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="D89" s="6">
-        <v>4904423</v>
+        <v>4904520</v>
       </c>
       <c r="E89" s="6">
-        <v>1211864</v>
+        <v>1212375</v>
       </c>
       <c r="F89" s="3">
         <v>1</v>
@@ -2871,43 +2935,43 @@
       </c>
     </row>
     <row r="90" spans="1:7">
-      <c r="A90" s="5">
-        <v>248</v>
-      </c>
-      <c r="B90" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C90" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="D90" s="7">
-        <v>4904649</v>
-      </c>
-      <c r="E90" s="7">
-        <v>1211985</v>
-      </c>
-      <c r="F90" s="2">
-        <v>1</v>
-      </c>
-      <c r="G90" s="2" t="s">
+      <c r="A90" s="4">
+        <v>351</v>
+      </c>
+      <c r="B90" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C90" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="D90" s="6">
+        <v>4903132</v>
+      </c>
+      <c r="E90" s="6">
+        <v>1210468</v>
+      </c>
+      <c r="F90" s="3">
+        <v>1</v>
+      </c>
+      <c r="G90" s="3" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="91" spans="1:7">
       <c r="A91" s="4">
-        <v>314</v>
+        <v>370</v>
       </c>
       <c r="B91" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C91" s="3" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="D91" s="6">
-        <v>4904349</v>
+        <v>4903528</v>
       </c>
       <c r="E91" s="6">
-        <v>1212388</v>
+        <v>1210646</v>
       </c>
       <c r="F91" s="3">
         <v>1</v>
@@ -2917,66 +2981,66 @@
       </c>
     </row>
     <row r="92" spans="1:7">
-      <c r="A92" s="5">
-        <v>58</v>
-      </c>
-      <c r="B92" s="2" t="s">
+      <c r="A92" s="4">
+        <v>371</v>
+      </c>
+      <c r="B92" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C92" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D92" s="6">
+        <v>4903653</v>
+      </c>
+      <c r="E92" s="6">
+        <v>1210666</v>
+      </c>
+      <c r="F92" s="3">
+        <v>1</v>
+      </c>
+      <c r="G92" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7">
+      <c r="A93" s="5">
+        <v>148</v>
+      </c>
+      <c r="B93" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C92" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="D92" s="7">
-        <v>4904685</v>
-      </c>
-      <c r="E92" s="7">
-        <v>1212198</v>
-      </c>
-      <c r="F92" s="2">
-        <v>4</v>
-      </c>
-      <c r="G92" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="93" spans="1:7">
-      <c r="A93" s="4">
-        <v>317</v>
-      </c>
-      <c r="B93" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C93" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="D93" s="6">
-        <v>4904520</v>
-      </c>
-      <c r="E93" s="6">
-        <v>1212375</v>
-      </c>
-      <c r="F93" s="3">
-        <v>1</v>
-      </c>
-      <c r="G93" s="3" t="s">
+      <c r="C93" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D93" s="7">
+        <v>4903631</v>
+      </c>
+      <c r="E93" s="7">
+        <v>1210513</v>
+      </c>
+      <c r="F93" s="2">
+        <v>1</v>
+      </c>
+      <c r="G93" s="2" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="94" spans="1:7">
       <c r="A94" s="4">
-        <v>351</v>
+        <v>372</v>
       </c>
       <c r="B94" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C94" s="3" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="D94" s="6">
-        <v>4903132</v>
+        <v>4903426</v>
       </c>
       <c r="E94" s="6">
-        <v>1210468</v>
+        <v>1210297</v>
       </c>
       <c r="F94" s="3">
         <v>1</v>
@@ -2987,19 +3051,19 @@
     </row>
     <row r="95" spans="1:7">
       <c r="A95" s="4">
-        <v>370</v>
+        <v>373</v>
       </c>
       <c r="B95" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C95" s="3" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="D95" s="6">
-        <v>4903528</v>
+        <v>4903678</v>
       </c>
       <c r="E95" s="6">
-        <v>1210646</v>
+        <v>1210269</v>
       </c>
       <c r="F95" s="3">
         <v>1</v>
@@ -3010,19 +3074,19 @@
     </row>
     <row r="96" spans="1:7">
       <c r="A96" s="4">
-        <v>371</v>
+        <v>309</v>
       </c>
       <c r="B96" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C96" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D96" s="6">
-        <v>4903653</v>
+        <v>4904223</v>
       </c>
       <c r="E96" s="6">
-        <v>1210666</v>
+        <v>1209977</v>
       </c>
       <c r="F96" s="3">
         <v>1</v>
@@ -3032,43 +3096,43 @@
       </c>
     </row>
     <row r="97" spans="1:7">
-      <c r="A97" s="5">
-        <v>148</v>
-      </c>
-      <c r="B97" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C97" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D97" s="7">
-        <v>4903631</v>
-      </c>
-      <c r="E97" s="7">
-        <v>1210513</v>
-      </c>
-      <c r="F97" s="2">
-        <v>1</v>
-      </c>
-      <c r="G97" s="2" t="s">
+      <c r="A97" s="4">
+        <v>308</v>
+      </c>
+      <c r="B97" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C97" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="D97" s="6">
+        <v>4904514</v>
+      </c>
+      <c r="E97" s="6">
+        <v>1210079</v>
+      </c>
+      <c r="F97" s="3">
+        <v>1</v>
+      </c>
+      <c r="G97" s="3" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="98" spans="1:7">
       <c r="A98" s="4">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="B98" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C98" s="3" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="D98" s="6">
-        <v>4903426</v>
+        <v>4903516</v>
       </c>
       <c r="E98" s="6">
-        <v>1210297</v>
+        <v>1211088</v>
       </c>
       <c r="F98" s="3">
         <v>1</v>
@@ -3079,19 +3143,19 @@
     </row>
     <row r="99" spans="1:7">
       <c r="A99" s="4">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="B99" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C99" s="3" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="D99" s="6">
-        <v>4903678</v>
+        <v>4903335</v>
       </c>
       <c r="E99" s="6">
-        <v>1210269</v>
+        <v>1210973</v>
       </c>
       <c r="F99" s="3">
         <v>1</v>
@@ -3101,66 +3165,66 @@
       </c>
     </row>
     <row r="100" spans="1:7">
-      <c r="A100" s="4">
-        <v>309</v>
-      </c>
-      <c r="B100" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C100" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D100" s="6">
-        <v>4904223</v>
-      </c>
-      <c r="E100" s="6">
-        <v>1209977</v>
-      </c>
-      <c r="F100" s="3">
-        <v>1</v>
-      </c>
-      <c r="G100" s="3" t="s">
+      <c r="A100" s="5">
+        <v>147</v>
+      </c>
+      <c r="B100" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C100" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="D100" s="7">
+        <v>4903138</v>
+      </c>
+      <c r="E100" s="7">
+        <v>1211546</v>
+      </c>
+      <c r="F100" s="2">
+        <v>1</v>
+      </c>
+      <c r="G100" s="2" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="101" spans="1:7">
-      <c r="A101" s="4">
-        <v>308</v>
-      </c>
-      <c r="B101" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C101" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="D101" s="6">
-        <v>4904514</v>
-      </c>
-      <c r="E101" s="6">
-        <v>1210079</v>
-      </c>
-      <c r="F101" s="3">
-        <v>1</v>
-      </c>
-      <c r="G101" s="3" t="s">
+      <c r="A101" s="5">
+        <v>160</v>
+      </c>
+      <c r="B101" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C101" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="D101" s="7">
+        <v>4903287</v>
+      </c>
+      <c r="E101" s="7">
+        <v>1211530</v>
+      </c>
+      <c r="F101" s="2">
+        <v>1</v>
+      </c>
+      <c r="G101" s="2" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="102" spans="1:7">
       <c r="A102" s="4">
-        <v>368</v>
+        <v>358</v>
       </c>
       <c r="B102" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C102" s="3" t="s">
-        <v>119</v>
+        <v>16</v>
       </c>
       <c r="D102" s="6">
-        <v>4903516</v>
+        <v>4903173</v>
       </c>
       <c r="E102" s="6">
-        <v>1211088</v>
+        <v>1212031</v>
       </c>
       <c r="F102" s="3">
         <v>1</v>
@@ -3171,19 +3235,19 @@
     </row>
     <row r="103" spans="1:7">
       <c r="A103" s="4">
-        <v>369</v>
+        <v>357</v>
       </c>
       <c r="B103" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C103" s="3" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="D103" s="6">
-        <v>4903335</v>
+        <v>4903034</v>
       </c>
       <c r="E103" s="6">
-        <v>1210973</v>
+        <v>1211873</v>
       </c>
       <c r="F103" s="3">
         <v>1</v>
@@ -3193,66 +3257,66 @@
       </c>
     </row>
     <row r="104" spans="1:7">
-      <c r="A104" s="5">
-        <v>147</v>
-      </c>
-      <c r="B104" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C104" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="D104" s="7">
-        <v>4903138</v>
-      </c>
-      <c r="E104" s="7">
-        <v>1211546</v>
-      </c>
-      <c r="F104" s="2">
-        <v>1</v>
-      </c>
-      <c r="G104" s="2" t="s">
+      <c r="A104" s="4">
+        <v>359</v>
+      </c>
+      <c r="B104" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C104" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="D104" s="6">
+        <v>4903052</v>
+      </c>
+      <c r="E104" s="6">
+        <v>1212090</v>
+      </c>
+      <c r="F104" s="3">
+        <v>1</v>
+      </c>
+      <c r="G104" s="3" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="105" spans="1:7">
-      <c r="A105" s="5">
-        <v>160</v>
-      </c>
-      <c r="B105" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C105" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="D105" s="7">
-        <v>4903287</v>
-      </c>
-      <c r="E105" s="7">
-        <v>1211530</v>
-      </c>
-      <c r="F105" s="2">
-        <v>1</v>
-      </c>
-      <c r="G105" s="2" t="s">
+      <c r="A105" s="4">
+        <v>377</v>
+      </c>
+      <c r="B105" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C105" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D105" s="6">
+        <v>4902343</v>
+      </c>
+      <c r="E105" s="6">
+        <v>1211290</v>
+      </c>
+      <c r="F105" s="3">
+        <v>1</v>
+      </c>
+      <c r="G105" s="3" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="106" spans="1:7">
       <c r="A106" s="4">
-        <v>358</v>
+        <v>382</v>
       </c>
       <c r="B106" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C106" s="3" t="s">
-        <v>16</v>
+        <v>125</v>
       </c>
       <c r="D106" s="6">
-        <v>4903173</v>
+        <v>4902366</v>
       </c>
       <c r="E106" s="6">
-        <v>1212031</v>
+        <v>1211700</v>
       </c>
       <c r="F106" s="3">
         <v>1</v>
@@ -3263,19 +3327,19 @@
     </row>
     <row r="107" spans="1:7">
       <c r="A107" s="4">
-        <v>357</v>
+        <v>383</v>
       </c>
       <c r="B107" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C107" s="3" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="D107" s="6">
-        <v>4903034</v>
+        <v>4902256</v>
       </c>
       <c r="E107" s="6">
-        <v>1211873</v>
+        <v>1211735</v>
       </c>
       <c r="F107" s="3">
         <v>1</v>
@@ -3286,19 +3350,19 @@
     </row>
     <row r="108" spans="1:7">
       <c r="A108" s="4">
-        <v>359</v>
+        <v>378</v>
       </c>
       <c r="B108" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C108" s="3" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="D108" s="6">
-        <v>4903052</v>
+        <v>4902653</v>
       </c>
       <c r="E108" s="6">
-        <v>1212090</v>
+        <v>1211940</v>
       </c>
       <c r="F108" s="3">
         <v>1</v>
@@ -3309,19 +3373,19 @@
     </row>
     <row r="109" spans="1:7">
       <c r="A109" s="4">
-        <v>377</v>
+        <v>379</v>
       </c>
       <c r="B109" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C109" s="3" t="s">
-        <v>17</v>
+        <v>128</v>
       </c>
       <c r="D109" s="6">
-        <v>4902343</v>
+        <v>4902513</v>
       </c>
       <c r="E109" s="6">
-        <v>1211290</v>
+        <v>1212271</v>
       </c>
       <c r="F109" s="3">
         <v>1</v>
@@ -3332,19 +3396,19 @@
     </row>
     <row r="110" spans="1:7">
       <c r="A110" s="4">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="B110" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C110" s="3" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="D110" s="6">
-        <v>4902366</v>
+        <v>4902449</v>
       </c>
       <c r="E110" s="6">
-        <v>1211700</v>
+        <v>1212180</v>
       </c>
       <c r="F110" s="3">
         <v>1</v>
@@ -3355,19 +3419,19 @@
     </row>
     <row r="111" spans="1:7">
       <c r="A111" s="4">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="B111" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C111" s="3" t="s">
-        <v>126</v>
+        <v>18</v>
       </c>
       <c r="D111" s="6">
-        <v>4902256</v>
+        <v>4902356</v>
       </c>
       <c r="E111" s="6">
-        <v>1211735</v>
+        <v>1212240</v>
       </c>
       <c r="F111" s="3">
         <v>1</v>
@@ -3378,19 +3442,19 @@
     </row>
     <row r="112" spans="1:7">
       <c r="A112" s="4">
-        <v>378</v>
+        <v>384</v>
       </c>
       <c r="B112" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C112" s="3" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="D112" s="6">
-        <v>4902653</v>
+        <v>4902805</v>
       </c>
       <c r="E112" s="6">
-        <v>1211940</v>
+        <v>1213110</v>
       </c>
       <c r="F112" s="3">
         <v>1</v>
@@ -3401,19 +3465,19 @@
     </row>
     <row r="113" spans="1:7">
       <c r="A113" s="4">
-        <v>379</v>
+        <v>355</v>
       </c>
       <c r="B113" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C113" s="3" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="D113" s="6">
-        <v>4902513</v>
+        <v>4902894</v>
       </c>
       <c r="E113" s="6">
-        <v>1212271</v>
+        <v>1211027</v>
       </c>
       <c r="F113" s="3">
         <v>1</v>
@@ -3424,19 +3488,19 @@
     </row>
     <row r="114" spans="1:7">
       <c r="A114" s="4">
-        <v>380</v>
+        <v>353</v>
       </c>
       <c r="B114" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C114" s="3" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="D114" s="6">
-        <v>4902449</v>
+        <v>4902883</v>
       </c>
       <c r="E114" s="6">
-        <v>1212180</v>
+        <v>1210627</v>
       </c>
       <c r="F114" s="3">
         <v>1</v>
@@ -3447,19 +3511,19 @@
     </row>
     <row r="115" spans="1:7">
       <c r="A115" s="4">
-        <v>381</v>
+        <v>352</v>
       </c>
       <c r="B115" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C115" s="3" t="s">
-        <v>18</v>
+        <v>133</v>
       </c>
       <c r="D115" s="6">
-        <v>4902356</v>
+        <v>4902978</v>
       </c>
       <c r="E115" s="6">
-        <v>1212240</v>
+        <v>1210398</v>
       </c>
       <c r="F115" s="3">
         <v>1</v>
@@ -3470,19 +3534,19 @@
     </row>
     <row r="116" spans="1:7">
       <c r="A116" s="4">
-        <v>384</v>
+        <v>356</v>
       </c>
       <c r="B116" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C116" s="3" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="D116" s="6">
-        <v>4902805</v>
+        <v>4902924</v>
       </c>
       <c r="E116" s="6">
-        <v>1213110</v>
+        <v>1211263</v>
       </c>
       <c r="F116" s="3">
         <v>1</v>
@@ -3493,19 +3557,19 @@
     </row>
     <row r="117" spans="1:7">
       <c r="A117" s="4">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B117" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C117" s="3" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="D117" s="6">
-        <v>4902894</v>
+        <v>4903027</v>
       </c>
       <c r="E117" s="6">
-        <v>1211027</v>
+        <v>1210857</v>
       </c>
       <c r="F117" s="3">
         <v>1</v>
@@ -3516,19 +3580,19 @@
     </row>
     <row r="118" spans="1:7">
       <c r="A118" s="4">
-        <v>353</v>
+        <v>400</v>
       </c>
       <c r="B118" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C118" s="3" t="s">
-        <v>132</v>
+        <v>19</v>
       </c>
       <c r="D118" s="6">
-        <v>4902883</v>
+        <v>4902992</v>
       </c>
       <c r="E118" s="6">
-        <v>1210627</v>
+        <v>1210116</v>
       </c>
       <c r="F118" s="3">
         <v>1</v>
@@ -3539,19 +3603,19 @@
     </row>
     <row r="119" spans="1:7">
       <c r="A119" s="4">
-        <v>352</v>
+        <v>374</v>
       </c>
       <c r="B119" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C119" s="3" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="D119" s="6">
-        <v>4902978</v>
+        <v>4902738</v>
       </c>
       <c r="E119" s="6">
-        <v>1210398</v>
+        <v>1210602</v>
       </c>
       <c r="F119" s="3">
         <v>1</v>
@@ -3562,19 +3626,19 @@
     </row>
     <row r="120" spans="1:7">
       <c r="A120" s="4">
-        <v>356</v>
+        <v>493</v>
       </c>
       <c r="B120" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C120" s="3" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="D120" s="6">
-        <v>4902924</v>
+        <v>4902508</v>
       </c>
       <c r="E120" s="6">
-        <v>1211263</v>
+        <v>1210878</v>
       </c>
       <c r="F120" s="3">
         <v>1</v>
@@ -3584,89 +3648,89 @@
       </c>
     </row>
     <row r="121" spans="1:7">
-      <c r="A121" s="4">
-        <v>354</v>
-      </c>
-      <c r="B121" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C121" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="D121" s="6">
-        <v>4903027</v>
-      </c>
-      <c r="E121" s="6">
-        <v>1210857</v>
-      </c>
-      <c r="F121" s="3">
-        <v>1</v>
-      </c>
-      <c r="G121" s="3" t="s">
+      <c r="A121" s="5">
+        <v>74</v>
+      </c>
+      <c r="B121" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C121" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="D121" s="7">
+        <v>4902597</v>
+      </c>
+      <c r="E121" s="7">
+        <v>1210637</v>
+      </c>
+      <c r="F121" s="2">
+        <v>1</v>
+      </c>
+      <c r="G121" s="2" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="122" spans="1:7">
-      <c r="A122" s="4">
-        <v>400</v>
-      </c>
-      <c r="B122" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C122" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D122" s="6">
-        <v>4902992</v>
-      </c>
-      <c r="E122" s="6">
-        <v>1210116</v>
-      </c>
-      <c r="F122" s="3">
-        <v>1</v>
-      </c>
-      <c r="G122" s="3" t="s">
+      <c r="A122" s="5">
+        <v>21</v>
+      </c>
+      <c r="B122" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C122" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="D122" s="7">
+        <v>4902474</v>
+      </c>
+      <c r="E122" s="7">
+        <v>1210871</v>
+      </c>
+      <c r="F122" s="2">
+        <v>1</v>
+      </c>
+      <c r="G122" s="2" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="123" spans="1:7">
-      <c r="A123" s="4">
-        <v>374</v>
-      </c>
-      <c r="B123" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C123" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="D123" s="6">
-        <v>4902738</v>
-      </c>
-      <c r="E123" s="6">
-        <v>1210602</v>
-      </c>
-      <c r="F123" s="3">
-        <v>1</v>
-      </c>
-      <c r="G123" s="3" t="s">
+      <c r="A123" s="5">
+        <v>301</v>
+      </c>
+      <c r="B123" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C123" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="D123" s="7">
+        <v>4902475</v>
+      </c>
+      <c r="E123" s="7">
+        <v>1210921</v>
+      </c>
+      <c r="F123" s="2">
+        <v>1</v>
+      </c>
+      <c r="G123" s="2" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="124" spans="1:7">
       <c r="A124" s="4">
-        <v>493</v>
+        <v>375</v>
       </c>
       <c r="B124" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C124" s="3" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="D124" s="6">
-        <v>4902508</v>
+        <v>4902640</v>
       </c>
       <c r="E124" s="6">
-        <v>1210878</v>
+        <v>1211003</v>
       </c>
       <c r="F124" s="3">
         <v>1</v>
@@ -3676,66 +3740,66 @@
       </c>
     </row>
     <row r="125" spans="1:7">
-      <c r="A125" s="5">
-        <v>74</v>
-      </c>
-      <c r="B125" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C125" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="D125" s="7">
-        <v>4902597</v>
-      </c>
-      <c r="E125" s="7">
-        <v>1210637</v>
-      </c>
-      <c r="F125" s="2">
-        <v>1</v>
-      </c>
-      <c r="G125" s="2" t="s">
+      <c r="A125" s="4">
+        <v>376</v>
+      </c>
+      <c r="B125" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C125" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="D125" s="6">
+        <v>4902582</v>
+      </c>
+      <c r="E125" s="6">
+        <v>1211134</v>
+      </c>
+      <c r="F125" s="3">
+        <v>1</v>
+      </c>
+      <c r="G125" s="3" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="126" spans="1:7">
-      <c r="A126" s="5">
-        <v>21</v>
-      </c>
-      <c r="B126" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C126" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="D126" s="7">
-        <v>4902474</v>
-      </c>
-      <c r="E126" s="7">
-        <v>1210871</v>
-      </c>
-      <c r="F126" s="2">
-        <v>1</v>
-      </c>
-      <c r="G126" s="2" t="s">
+      <c r="A126" s="4">
+        <v>324</v>
+      </c>
+      <c r="B126" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C126" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D126" s="6">
+        <v>4903827</v>
+      </c>
+      <c r="E126" s="6">
+        <v>1213593</v>
+      </c>
+      <c r="F126" s="3">
+        <v>1</v>
+      </c>
+      <c r="G126" s="3" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="127" spans="1:7">
       <c r="A127" s="5">
-        <v>301</v>
+        <v>164</v>
       </c>
       <c r="B127" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C127" s="2" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="D127" s="7">
-        <v>4902475</v>
+        <v>4903933</v>
       </c>
       <c r="E127" s="7">
-        <v>1210921</v>
+        <v>1215718</v>
       </c>
       <c r="F127" s="2">
         <v>1</v>
@@ -3746,19 +3810,19 @@
     </row>
     <row r="128" spans="1:7">
       <c r="A128" s="4">
-        <v>375</v>
+        <v>349</v>
       </c>
       <c r="B128" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C128" s="3" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="D128" s="6">
-        <v>4902640</v>
+        <v>4904570</v>
       </c>
       <c r="E128" s="6">
-        <v>1211003</v>
+        <v>1216103</v>
       </c>
       <c r="F128" s="3">
         <v>1</v>
@@ -3769,19 +3833,19 @@
     </row>
     <row r="129" spans="1:7">
       <c r="A129" s="4">
-        <v>376</v>
+        <v>278</v>
       </c>
       <c r="B129" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C129" s="3" t="s">
-        <v>142</v>
+        <v>152</v>
       </c>
       <c r="D129" s="6">
-        <v>4902582</v>
+        <v>4902360</v>
       </c>
       <c r="E129" s="6">
-        <v>1211134</v>
+        <v>1214995</v>
       </c>
       <c r="F129" s="3">
         <v>1</v>
@@ -3792,19 +3856,19 @@
     </row>
     <row r="130" spans="1:7">
       <c r="A130" s="4">
-        <v>324</v>
+        <v>348</v>
       </c>
       <c r="B130" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C130" s="3" t="s">
-        <v>20</v>
+        <v>153</v>
       </c>
       <c r="D130" s="6">
-        <v>4903827</v>
+        <v>4904087</v>
       </c>
       <c r="E130" s="6">
-        <v>1213593</v>
+        <v>1216095</v>
       </c>
       <c r="F130" s="3">
         <v>1</v>
@@ -3814,43 +3878,43 @@
       </c>
     </row>
     <row r="131" spans="1:7">
-      <c r="A131" s="5">
-        <v>164</v>
-      </c>
-      <c r="B131" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C131" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="D131" s="7">
-        <v>4903933</v>
-      </c>
-      <c r="E131" s="7">
-        <v>1215718</v>
-      </c>
-      <c r="F131" s="2">
-        <v>1</v>
-      </c>
-      <c r="G131" s="2" t="s">
+      <c r="A131" s="4">
+        <v>346</v>
+      </c>
+      <c r="B131" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C131" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D131" s="6">
+        <v>4903969</v>
+      </c>
+      <c r="E131" s="6">
+        <v>1215234</v>
+      </c>
+      <c r="F131" s="3">
+        <v>1</v>
+      </c>
+      <c r="G131" s="3" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="132" spans="1:7">
       <c r="A132" s="4">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B132" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C132" s="3" t="s">
-        <v>144</v>
+        <v>22</v>
       </c>
       <c r="D132" s="6">
-        <v>4904570</v>
+        <v>4903811</v>
       </c>
       <c r="E132" s="6">
-        <v>1216103</v>
+        <v>1215843</v>
       </c>
       <c r="F132" s="3">
         <v>1</v>
@@ -3861,19 +3925,19 @@
     </row>
     <row r="133" spans="1:7">
       <c r="A133" s="4">
-        <v>278</v>
+        <v>146</v>
       </c>
       <c r="B133" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C133" s="3" t="s">
-        <v>152</v>
+        <v>23</v>
       </c>
       <c r="D133" s="6">
-        <v>4902360</v>
+        <v>4899082</v>
       </c>
       <c r="E133" s="6">
-        <v>1214995</v>
+        <v>1213627</v>
       </c>
       <c r="F133" s="3">
         <v>1</v>
@@ -3884,19 +3948,19 @@
     </row>
     <row r="134" spans="1:7">
       <c r="A134" s="4">
-        <v>348</v>
+        <v>475</v>
       </c>
       <c r="B134" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C134" s="3" t="s">
-        <v>153</v>
+        <v>24</v>
       </c>
       <c r="D134" s="6">
-        <v>4904087</v>
+        <v>4904181</v>
       </c>
       <c r="E134" s="6">
-        <v>1216095</v>
+        <v>1215529</v>
       </c>
       <c r="F134" s="3">
         <v>1</v>
@@ -3907,19 +3971,19 @@
     </row>
     <row r="135" spans="1:7">
       <c r="A135" s="4">
-        <v>346</v>
+        <v>350</v>
       </c>
       <c r="B135" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C135" s="3" t="s">
-        <v>21</v>
+        <v>145</v>
       </c>
       <c r="D135" s="6">
-        <v>4903969</v>
+        <v>4904464</v>
       </c>
       <c r="E135" s="6">
-        <v>1215234</v>
+        <v>1215846</v>
       </c>
       <c r="F135" s="3">
         <v>1</v>
@@ -3930,19 +3994,19 @@
     </row>
     <row r="136" spans="1:7">
       <c r="A136" s="4">
-        <v>347</v>
+        <v>280</v>
       </c>
       <c r="B136" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C136" s="3" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D136" s="6">
-        <v>4903811</v>
+        <v>4902138</v>
       </c>
       <c r="E136" s="6">
-        <v>1215843</v>
+        <v>1215435</v>
       </c>
       <c r="F136" s="3">
         <v>1</v>
@@ -3953,19 +4017,19 @@
     </row>
     <row r="137" spans="1:7">
       <c r="A137" s="4">
-        <v>146</v>
+        <v>285</v>
       </c>
       <c r="B137" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C137" s="3" t="s">
-        <v>23</v>
+        <v>154</v>
       </c>
       <c r="D137" s="6">
-        <v>4899082</v>
+        <v>4902674</v>
       </c>
       <c r="E137" s="6">
-        <v>1213627</v>
+        <v>1215423</v>
       </c>
       <c r="F137" s="3">
         <v>1</v>
@@ -3976,19 +4040,19 @@
     </row>
     <row r="138" spans="1:7">
       <c r="A138" s="4">
-        <v>475</v>
+        <v>282</v>
       </c>
       <c r="B138" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C138" s="3" t="s">
-        <v>24</v>
+        <v>146</v>
       </c>
       <c r="D138" s="6">
-        <v>4904181</v>
+        <v>4902423</v>
       </c>
       <c r="E138" s="6">
-        <v>1215529</v>
+        <v>1215260</v>
       </c>
       <c r="F138" s="3">
         <v>1</v>
@@ -3999,19 +4063,19 @@
     </row>
     <row r="139" spans="1:7">
       <c r="A139" s="4">
-        <v>350</v>
+        <v>281</v>
       </c>
       <c r="B139" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C139" s="3" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="D139" s="6">
-        <v>4904464</v>
+        <v>4902317</v>
       </c>
       <c r="E139" s="6">
-        <v>1215846</v>
+        <v>1215530</v>
       </c>
       <c r="F139" s="3">
         <v>1</v>
@@ -4022,19 +4086,19 @@
     </row>
     <row r="140" spans="1:7">
       <c r="A140" s="4">
-        <v>280</v>
+        <v>286</v>
       </c>
       <c r="B140" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C140" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D140" s="6">
-        <v>4902138</v>
+        <v>4902662</v>
       </c>
       <c r="E140" s="6">
-        <v>1215435</v>
+        <v>1215170</v>
       </c>
       <c r="F140" s="3">
         <v>1</v>
@@ -4045,19 +4109,19 @@
     </row>
     <row r="141" spans="1:7">
       <c r="A141" s="4">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B141" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C141" s="3" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="D141" s="6">
-        <v>4902674</v>
+        <v>4902532</v>
       </c>
       <c r="E141" s="6">
-        <v>1215423</v>
+        <v>1215658</v>
       </c>
       <c r="F141" s="3">
         <v>1</v>
@@ -4068,19 +4132,19 @@
     </row>
     <row r="142" spans="1:7">
       <c r="A142" s="4">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="B142" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C142" s="3" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="D142" s="6">
-        <v>4902423</v>
+        <v>4902507</v>
       </c>
       <c r="E142" s="6">
-        <v>1215260</v>
+        <v>1215271</v>
       </c>
       <c r="F142" s="3">
         <v>1</v>
@@ -4091,19 +4155,19 @@
     </row>
     <row r="143" spans="1:7">
       <c r="A143" s="4">
-        <v>281</v>
+        <v>456</v>
       </c>
       <c r="B143" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C143" s="3" t="s">
-        <v>147</v>
+        <v>155</v>
       </c>
       <c r="D143" s="6">
-        <v>4902317</v>
+        <v>4902608</v>
       </c>
       <c r="E143" s="6">
-        <v>1215530</v>
+        <v>1214817</v>
       </c>
       <c r="F143" s="3">
         <v>1</v>
@@ -4114,19 +4178,19 @@
     </row>
     <row r="144" spans="1:7">
       <c r="A144" s="4">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="B144" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C144" s="3" t="s">
-        <v>26</v>
+        <v>156</v>
       </c>
       <c r="D144" s="6">
-        <v>4902662</v>
+        <v>4902611</v>
       </c>
       <c r="E144" s="6">
-        <v>1215170</v>
+        <v>1214866</v>
       </c>
       <c r="F144" s="3">
         <v>1</v>
@@ -4137,19 +4201,19 @@
     </row>
     <row r="145" spans="1:7">
       <c r="A145" s="4">
-        <v>284</v>
+        <v>279</v>
       </c>
       <c r="B145" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C145" s="3" t="s">
-        <v>148</v>
+        <v>157</v>
       </c>
       <c r="D145" s="6">
-        <v>4902532</v>
+        <v>4902191</v>
       </c>
       <c r="E145" s="6">
-        <v>1215658</v>
+        <v>1215127</v>
       </c>
       <c r="F145" s="3">
         <v>1</v>
@@ -4160,19 +4224,19 @@
     </row>
     <row r="146" spans="1:7">
       <c r="A146" s="4">
-        <v>283</v>
+        <v>277</v>
       </c>
       <c r="B146" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C146" s="3" t="s">
-        <v>149</v>
+        <v>158</v>
       </c>
       <c r="D146" s="6">
-        <v>4902507</v>
+        <v>4902289</v>
       </c>
       <c r="E146" s="6">
-        <v>1215271</v>
+        <v>1214839</v>
       </c>
       <c r="F146" s="3">
         <v>1</v>
@@ -4182,43 +4246,43 @@
       </c>
     </row>
     <row r="147" spans="1:7">
-      <c r="A147" s="4">
-        <v>456</v>
-      </c>
-      <c r="B147" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C147" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="D147" s="6">
-        <v>4902608</v>
-      </c>
-      <c r="E147" s="6">
-        <v>1214817</v>
-      </c>
-      <c r="F147" s="3">
-        <v>1</v>
-      </c>
-      <c r="G147" s="3" t="s">
+      <c r="A147" s="5">
+        <v>112</v>
+      </c>
+      <c r="B147" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C147" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="D147" s="7">
+        <v>4902375</v>
+      </c>
+      <c r="E147" s="7">
+        <v>1214595</v>
+      </c>
+      <c r="F147" s="2">
+        <v>1</v>
+      </c>
+      <c r="G147" s="2" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="148" spans="1:7">
       <c r="A148" s="4">
-        <v>288</v>
+        <v>276</v>
       </c>
       <c r="B148" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C148" s="3" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="D148" s="6">
-        <v>4902611</v>
+        <v>4902405</v>
       </c>
       <c r="E148" s="6">
-        <v>1214866</v>
+        <v>1214564</v>
       </c>
       <c r="F148" s="3">
         <v>1</v>
@@ -4229,19 +4293,19 @@
     </row>
     <row r="149" spans="1:7">
       <c r="A149" s="4">
-        <v>279</v>
+        <v>287</v>
       </c>
       <c r="B149" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C149" s="3" t="s">
-        <v>157</v>
+        <v>27</v>
       </c>
       <c r="D149" s="6">
-        <v>4902191</v>
+        <v>4902540</v>
       </c>
       <c r="E149" s="6">
-        <v>1215127</v>
+        <v>1215100</v>
       </c>
       <c r="F149" s="3">
         <v>1</v>
@@ -4252,19 +4316,19 @@
     </row>
     <row r="150" spans="1:7">
       <c r="A150" s="4">
-        <v>277</v>
+        <v>294</v>
       </c>
       <c r="B150" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C150" s="3" t="s">
-        <v>158</v>
+        <v>28</v>
       </c>
       <c r="D150" s="6">
-        <v>4902289</v>
+        <v>4906547</v>
       </c>
       <c r="E150" s="6">
-        <v>1214839</v>
+        <v>1211659</v>
       </c>
       <c r="F150" s="3">
         <v>1</v>
@@ -4274,117 +4338,25 @@
       </c>
     </row>
     <row r="151" spans="1:7">
-      <c r="A151" s="5">
-        <v>112</v>
-      </c>
-      <c r="B151" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C151" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="D151" s="7">
-        <v>4902375</v>
-      </c>
-      <c r="E151" s="7">
-        <v>1214595</v>
-      </c>
-      <c r="F151" s="2">
-        <v>1</v>
-      </c>
-      <c r="G151" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="152" spans="1:7">
-      <c r="A152" s="4">
-        <v>276</v>
-      </c>
-      <c r="B152" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C152" s="3" t="s">
-        <v>150</v>
-      </c>
-      <c r="D152" s="6">
-        <v>4902405</v>
-      </c>
-      <c r="E152" s="6">
-        <v>1214564</v>
-      </c>
-      <c r="F152" s="3">
-        <v>1</v>
-      </c>
-      <c r="G152" s="3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="153" spans="1:7">
-      <c r="A153" s="4">
-        <v>287</v>
-      </c>
-      <c r="B153" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C153" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D153" s="6">
-        <v>4902540</v>
-      </c>
-      <c r="E153" s="6">
-        <v>1215100</v>
-      </c>
-      <c r="F153" s="3">
-        <v>1</v>
-      </c>
-      <c r="G153" s="3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="154" spans="1:7">
-      <c r="A154" s="4">
-        <v>294</v>
-      </c>
-      <c r="B154" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C154" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D154" s="6">
-        <v>4906547</v>
-      </c>
-      <c r="E154" s="6">
-        <v>1211659</v>
-      </c>
-      <c r="F154" s="3">
-        <v>1</v>
-      </c>
-      <c r="G154" s="3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="155" spans="1:7">
-      <c r="A155" s="4">
+      <c r="A151" s="4">
         <v>293</v>
       </c>
-      <c r="B155" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C155" s="3" t="s">
+      <c r="B151" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C151" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="D155" s="6">
+      <c r="D151" s="6">
         <v>4906394</v>
       </c>
-      <c r="E155" s="6">
+      <c r="E151" s="6">
         <v>1211995</v>
       </c>
-      <c r="F155" s="3">
-        <v>1</v>
-      </c>
-      <c r="G155" s="3" t="s">
+      <c r="F151" s="3">
+        <v>1</v>
+      </c>
+      <c r="G151" s="3" t="s">
         <v>0</v>
       </c>
     </row>

</xml_diff>